<commit_message>
fix page show discount function
</commit_message>
<xml_diff>
--- a/form/static/病理切片校外含稅 v3.1.xlsx
+++ b/form/static/病理切片校外含稅 v3.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\手開帳單原檔\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\ntucmform\ntucmlac_form\ntucmlab_userform\form\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04F0F5B-57EC-449A-BF44-4E63479BE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9861E0B-3DB5-4DA7-92BB-910AA91EF68C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,6 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -464,46 +455,46 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -873,38 +864,38 @@
   </sheetPr>
   <dimension ref="A1:IW46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="84" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="84" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="16.25" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.75" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22.375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="9" style="6" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="0.125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="0.109375" style="6" customWidth="1"/>
     <col min="9" max="257" width="9" style="6" customWidth="1"/>
     <col min="258" max="1025" width="9" style="12" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="27.75">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="25.5">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="28.2">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="24.6">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -912,52 +903,52 @@
       <c r="E2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
       <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="19.5">
+    <row r="4" spans="1:8" ht="19.8">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="19.5">
+    <row r="6" spans="1:8" ht="19.8">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:8" ht="19.5">
+    <row r="7" spans="1:8" ht="19.8">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
@@ -966,244 +957,244 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="19.5">
+    <row r="9" spans="1:8" ht="19.8">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:8" ht="19.5">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:8" ht="19.8">
+      <c r="A10" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="14" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="36"/>
-    </row>
-    <row r="11" spans="1:8" ht="19.5">
-      <c r="A11" s="30" t="s">
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:8" ht="19.8">
+      <c r="A11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="15">
         <v>0</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="33">
         <f>70*E11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="34"/>
-    </row>
-    <row r="12" spans="1:8" ht="19.5">
-      <c r="A12" s="30" t="s">
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="1:8" ht="19.8">
+      <c r="A12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="14">
         <v>0</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="33">
         <f>70*E12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="34"/>
-    </row>
-    <row r="13" spans="1:8" ht="19.5">
-      <c r="A13" s="30" t="s">
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="1:8" ht="19.8">
+      <c r="A13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="14">
         <v>0</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="34">
         <f>85*E13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="31"/>
-    </row>
-    <row r="14" spans="1:8" ht="19.5">
-      <c r="A14" s="30" t="s">
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:8" ht="19.8">
+      <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="14">
         <v>0</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="33">
         <f>70*E14</f>
         <v>0</v>
       </c>
-      <c r="G14" s="34"/>
-    </row>
-    <row r="15" spans="1:8" ht="19.5">
-      <c r="A15" s="30" t="s">
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:8" ht="19.8">
+      <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="14">
         <v>0</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="34">
         <f>215*E15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="31"/>
-    </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" ht="19.5">
-      <c r="A16" s="30" t="s">
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="19.8">
+      <c r="A16" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="14">
         <v>0</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="33">
         <f>140*E16</f>
         <v>0</v>
       </c>
-      <c r="G16" s="34"/>
-    </row>
-    <row r="17" spans="1:257" ht="19.5">
-      <c r="A17" s="30" t="s">
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" spans="1:257" ht="19.8">
+      <c r="A17" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="14">
         <v>0</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="33">
         <f>85*E17</f>
         <v>0</v>
       </c>
-      <c r="G17" s="34"/>
-    </row>
-    <row r="18" spans="1:257" ht="19.5">
-      <c r="A18" s="30" t="s">
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="1:257" ht="19.8">
+      <c r="A18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="14">
         <v>0</v>
       </c>
-      <c r="F18" s="34">
+      <c r="F18" s="33">
         <f>E18*140</f>
         <v>0</v>
       </c>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" spans="1:257" ht="19.5">
-      <c r="A19" s="30" t="s">
+      <c r="G18" s="33"/>
+    </row>
+    <row r="19" spans="1:257" ht="19.8">
+      <c r="A19" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="14" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="14">
         <v>0</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="33">
         <f>850*E19</f>
         <v>0</v>
       </c>
-      <c r="G19" s="34"/>
-    </row>
-    <row r="20" spans="1:257" ht="19.5">
-      <c r="A20" s="30" t="s">
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="1:257" ht="19.8">
+      <c r="A20" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="15" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="15">
         <v>0</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="33">
         <f>200*E20</f>
         <v>0</v>
       </c>
-      <c r="G20" s="34"/>
-    </row>
-    <row r="21" spans="1:257" ht="19.5">
-      <c r="A21" s="30" t="s">
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:257" ht="19.8">
+      <c r="A21" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E21" s="15">
         <v>0</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="34">
         <f>200*E21</f>
         <v>0</v>
       </c>
-      <c r="G21" s="31"/>
-    </row>
-    <row r="22" spans="1:257" ht="19.5">
-      <c r="A22" s="30" t="s">
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:257" ht="19.8">
+      <c r="A22" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E22" s="15">
         <v>0</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="34">
         <f>200*E22</f>
         <v>0</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
@@ -1455,7 +1446,7 @@
       <c r="IV22" s="24"/>
       <c r="IW22" s="24"/>
     </row>
-    <row r="23" spans="1:257" ht="19.5">
+    <row r="23" spans="1:257" ht="19.8">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1464,12 +1455,12 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="1:257" ht="19.5">
-      <c r="A24" s="33" t="s">
+    <row r="24" spans="1:257" ht="19.8">
+      <c r="A24" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="26">
         <f>SUM(F11:G22)</f>
         <v>0</v>
@@ -1728,12 +1719,12 @@
       <c r="IV24" s="25"/>
       <c r="IW24" s="25"/>
     </row>
-    <row r="25" spans="1:257" ht="19.5">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:257" ht="19.8">
+      <c r="A25" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="26">
         <f>ROUND(D24*0.05,0)</f>
         <v>0</v>
@@ -1992,21 +1983,21 @@
       <c r="IV25" s="25"/>
       <c r="IW25" s="25"/>
     </row>
-    <row r="26" spans="1:257" ht="19.5">
-      <c r="A26" s="32" t="s">
+    <row r="26" spans="1:257" ht="19.8">
+      <c r="A26" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="8">
-        <f>SUM(F11:G22)</f>
+        <f>SUM(D24:D25)</f>
         <v>0</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="1:257" ht="19.5">
+    <row r="27" spans="1:257" ht="19.8">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -2015,214 +2006,186 @@
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="1:257" ht="25.7" customHeight="1">
+    <row r="28" spans="1:257" ht="25.65" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
     </row>
     <row r="29" spans="1:257" ht="16.5" customHeight="1">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
     </row>
     <row r="30" spans="1:257">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" spans="1:257">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" spans="1:257">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" spans="1:7" ht="79.5" customHeight="1">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange password="CAA6" sqref="F24:G25" name="總價"/>
   </protectedRanges>
   <mergeCells count="37">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="F20:G20"/>
     <mergeCell ref="A29:G46"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="F21:G21"/>
@@ -2232,6 +2195,34 @@
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74861111111111101" header="0.51180555555555496" footer="0.31527777777777799"/>

</xml_diff>